<commit_message>
LPNI transition report corrected text
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@3094 ef391c1c-ee15-45f7-b1d6-dde3d27a2169

Former-commit-id: 1c6c29fbf0e089131877b59b879246d8ba752d78
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_LPNI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_LPNI_Transition_Report_Template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
@@ -219,11 +219,6 @@
     <t>Report Overview</t>
   </si>
   <si>
-    <t>The Office of Transition Management (OTM) Transition Application Planning (TAP) coordinated with the Defense Health Clinical Systems (DHCS) and Defense Health Services Systems (DHSS) program offices, in addition to the tri-Services, to collect technical and functional data regarding their information systems, in order to fully characterize the legacy DHA IM/IT portfolio. 
-Using this data, OTM provided detailed analysis regarding each legacy system to the Functional Advisory Council (FAC), which made transition decisions that define if each system would be replaced by the future-state EHR (high probability systems) or would endure to support the future-state EHR (low probability systems).
-This report focuses on low probability systems that will require integration with the future-state EHR and provides analytical insights that specify the activities required for the system highlighted in this report to transition to the future state environment.</t>
-  </si>
-  <si>
     <t>Direct Cost</t>
   </si>
   <si>
@@ -394,6 +389,11 @@
   </si>
   <si>
     <t>This section displays the data objects that @SYSTEM@ is a source of record of and consumes. For each data object @SYSTEM@ is a source of record of, the number in the @SYSTEM@ column represents the number of systems the data object is passed to. For each data object @SYSTEM@ consumes, the highlighted cells depict the systems @SYSTEM@ receives the data from. The numbers in these cells represent the total number of systems they pass the data objects to.</t>
+  </si>
+  <si>
+    <t>The Office of Transition Management (OTM) Transition Application Planning (TAP) coordinated with the Defense Health Clinical Systems (DHCS) and Defense Health Services Systems (DHSS) program offices, in addition to the tri-Services, to collect technical and functional data regarding their information systems, in order to fully characterize the legacy DHA IM/IT portfolio. 
+Using this data, OTM provided detailed analysis regarding each legacy system to the Functional Advisory Council (FAC), which made transition decisions that define if each system would be replaced by the future-state EHR (high probability systems) or would endure to support the future-state EHR (low probability systems).
+This report focuses on low probability systems that will not require integration with the future-state EHR and provides analytical insights that specify the activities required for the system highlighted in this report to transition to the future state environment.</t>
   </si>
 </sst>
 </file>
@@ -976,33 +976,6 @@
     <xf numFmtId="0" fontId="24" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1030,6 +1003,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1039,10 +1021,28 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1412,11 +1412,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="553333016"/>
-        <c:axId val="553333408"/>
+        <c:axId val="381745528"/>
+        <c:axId val="381745920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="553333016"/>
+        <c:axId val="381745528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1426,7 +1426,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="553333408"/>
+        <c:crossAx val="381745920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1434,7 +1434,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="553333408"/>
+        <c:axId val="381745920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1445,7 +1445,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="553333016"/>
+        <c:crossAx val="381745528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1578,11 +1578,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="553334192"/>
-        <c:axId val="553334584"/>
+        <c:axId val="381746704"/>
+        <c:axId val="381747096"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="553334192"/>
+        <c:axId val="381746704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1592,7 +1592,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="553334584"/>
+        <c:crossAx val="381747096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1600,7 +1600,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="553334584"/>
+        <c:axId val="381747096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1611,7 +1611,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="553334192"/>
+        <c:crossAx val="381746704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1892,11 +1892,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="553335368"/>
-        <c:axId val="553335760"/>
+        <c:axId val="381747880"/>
+        <c:axId val="381748272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="553335368"/>
+        <c:axId val="381747880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1906,7 +1906,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="553335760"/>
+        <c:crossAx val="381748272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1914,7 +1914,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="553335760"/>
+        <c:axId val="381748272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1925,7 +1925,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="553335368"/>
+        <c:crossAx val="381747880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -44461,7 +44461,7 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:L4"/>
     </sheetView>
   </sheetViews>
@@ -44475,12 +44475,12 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="32.25" customHeight="1">
       <c r="A2" s="50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="51"/>
       <c r="C2" s="51"/>
@@ -44496,12 +44496,12 @@
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="286.5" customHeight="1">
       <c r="A4" s="52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="53"/>
       <c r="C4" s="53"/>
@@ -44517,12 +44517,12 @@
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="30" customFormat="1" ht="29.25" customHeight="1">
       <c r="A6" s="50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="51"/>
       <c r="C6" s="51"/>
@@ -44538,12 +44538,12 @@
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="7.5" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="134.25" customHeight="1">
       <c r="A8" s="55" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="56"/>
       <c r="C8" s="56"/>
@@ -44637,8 +44637,8 @@
   </sheetPr>
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q44" sqref="Q44"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44658,22 +44658,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="60" t="s">
-        <v>36</v>
+      <c r="C2" s="79"/>
+      <c r="D2" s="67" t="s">
+        <v>83</v>
       </c>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="61"/>
-      <c r="M2" s="62"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="69"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -44731,22 +44731,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="375" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="58" t="s">
+      <c r="B7" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="59"/>
-      <c r="D7" s="60" t="s">
-        <v>51</v>
+      <c r="C7" s="79"/>
+      <c r="D7" s="67" t="s">
+        <v>50</v>
       </c>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61"/>
-      <c r="L7" s="61"/>
-      <c r="M7" s="62"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="68"/>
+      <c r="L7" s="68"/>
+      <c r="M7" s="69"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -44757,112 +44757,112 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="68"/>
-      <c r="K9" s="68"/>
-      <c r="L9" s="68"/>
-      <c r="M9" s="69"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="59"/>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
+      <c r="M9" s="60"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="63" t="s">
+      <c r="B10" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63" t="s">
+      <c r="C10" s="73"/>
+      <c r="D10" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="66"/>
-      <c r="F10" s="63" t="s">
+      <c r="E10" s="80"/>
+      <c r="F10" s="73" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="73"/>
+      <c r="H10" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="63"/>
-      <c r="H10" s="79" t="s">
+      <c r="I10" s="75"/>
+      <c r="J10" s="73" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="80"/>
-      <c r="J10" s="63" t="s">
-        <v>41</v>
-      </c>
-      <c r="K10" s="63"/>
-      <c r="L10" s="63" t="s">
+      <c r="K10" s="73"/>
+      <c r="L10" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="63"/>
+      <c r="M10" s="73"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="64"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="65"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="64"/>
-      <c r="K11" s="65"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="65"/>
+      <c r="B11" s="76"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="76"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="77"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="77"/>
     </row>
     <row r="13" spans="1:13" ht="16.5">
-      <c r="B13" s="67" t="s">
-        <v>52</v>
+      <c r="B13" s="58" t="s">
+        <v>51</v>
       </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="68"/>
-      <c r="F13" s="68"/>
-      <c r="G13" s="68"/>
-      <c r="H13" s="68"/>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="68"/>
-      <c r="L13" s="68"/>
-      <c r="M13" s="69"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59"/>
+      <c r="J13" s="59"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="60"/>
     </row>
     <row r="14" spans="1:13" ht="51" customHeight="1">
-      <c r="B14" s="73" t="s">
-        <v>69</v>
+      <c r="B14" s="64" t="s">
+        <v>68</v>
       </c>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="74"/>
-      <c r="I14" s="74"/>
-      <c r="J14" s="74"/>
-      <c r="K14" s="74"/>
-      <c r="L14" s="74"/>
-      <c r="M14" s="75"/>
+      <c r="C14" s="65"/>
+      <c r="D14" s="65"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="65"/>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="66"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="B15" s="76" t="s">
-        <v>55</v>
+      <c r="B15" s="70" t="s">
+        <v>54</v>
       </c>
-      <c r="C15" s="77"/>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="78"/>
-      <c r="H15" s="76" t="s">
-        <v>61</v>
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="70" t="s">
+        <v>60</v>
       </c>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
-      <c r="K15" s="77"/>
-      <c r="L15" s="77"/>
-      <c r="M15" s="78"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="71"/>
+      <c r="K15" s="71"/>
+      <c r="L15" s="71"/>
+      <c r="M15" s="72"/>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="40"/>
@@ -45089,36 +45089,36 @@
       <c r="M31" s="48"/>
     </row>
     <row r="33" spans="2:13" ht="16.5">
-      <c r="B33" s="67" t="s">
-        <v>62</v>
+      <c r="B33" s="58" t="s">
+        <v>61</v>
       </c>
-      <c r="C33" s="68"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="68"/>
-      <c r="F33" s="68"/>
-      <c r="G33" s="68"/>
-      <c r="H33" s="68"/>
-      <c r="I33" s="68"/>
-      <c r="J33" s="68"/>
-      <c r="K33" s="68"/>
-      <c r="L33" s="68"/>
-      <c r="M33" s="69"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="59"/>
+      <c r="K33" s="59"/>
+      <c r="L33" s="59"/>
+      <c r="M33" s="60"/>
     </row>
     <row r="34" spans="2:13" ht="33.75" customHeight="1">
-      <c r="B34" s="70" t="s">
-        <v>68</v>
+      <c r="B34" s="61" t="s">
+        <v>67</v>
       </c>
-      <c r="C34" s="71"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="71"/>
-      <c r="F34" s="71"/>
-      <c r="G34" s="71"/>
-      <c r="H34" s="71"/>
-      <c r="I34" s="71"/>
-      <c r="J34" s="71"/>
-      <c r="K34" s="71"/>
-      <c r="L34" s="71"/>
-      <c r="M34" s="72"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="62"/>
+      <c r="J34" s="62"/>
+      <c r="K34" s="62"/>
+      <c r="L34" s="62"/>
+      <c r="M34" s="63"/>
     </row>
     <row r="35" spans="2:13">
       <c r="B35" s="40"/>
@@ -45346,17 +45346,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="D2:M2"/>
@@ -45370,6 +45359,17 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45404,7 +45404,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18" customHeight="1">
@@ -45431,12 +45431,12 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="67.5" customHeight="1">
       <c r="A5" s="88" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="89"/>
       <c r="C5" s="89"/>
@@ -45447,7 +45447,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18.75" customHeight="1">
@@ -45456,7 +45456,7 @@
       </c>
       <c r="B7" s="86"/>
       <c r="C7" s="82" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="83"/>
       <c r="E7" s="83"/>
@@ -45465,7 +45465,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="25.5">
@@ -45473,7 +45473,7 @@
         <v>16</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="33" t="s">
         <v>27</v>
@@ -45502,7 +45502,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -45567,7 +45567,7 @@
     </row>
     <row r="5" spans="1:7" ht="67.5" customHeight="1">
       <c r="A5" s="88" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="89"/>
       <c r="C5" s="89"/>
@@ -45582,7 +45582,7 @@
       </c>
       <c r="B7" s="87"/>
       <c r="C7" s="94" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7" s="94"/>
       <c r="E7" s="94"/>
@@ -45594,7 +45594,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C9" s="33" t="s">
         <v>27</v>
@@ -45675,7 +45675,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="96" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="97"/>
       <c r="D4" s="97"/>
@@ -45691,7 +45691,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -45730,7 +45730,7 @@
   <sheetData>
     <row r="2" spans="1:2" ht="18">
       <c r="A2" s="95" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="95"/>
     </row>
@@ -45809,7 +45809,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="99" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C4" s="100"/>
     </row>
@@ -45826,7 +45826,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -45900,7 +45900,7 @@
       <c r="B4" s="102"/>
       <c r="C4" s="103"/>
       <c r="D4" s="104" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="105"/>
       <c r="F4" s="105"/>
@@ -45914,22 +45914,22 @@
     </row>
     <row r="6" spans="1:13" ht="96.75" customHeight="1">
       <c r="A6" s="108" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" s="49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="107"/>
       <c r="D6" s="107"/>
       <c r="E6" s="107"/>
       <c r="F6" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G6" s="107"/>
       <c r="H6" s="107"/>
       <c r="I6" s="107"/>
       <c r="J6" s="49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K6" s="107"/>
       <c r="L6" s="107"/>
@@ -45938,7 +45938,7 @@
     <row r="7" spans="1:13" ht="45" customHeight="1">
       <c r="A7" s="108"/>
       <c r="B7" s="49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" s="109"/>
       <c r="D7" s="110"/>
@@ -45978,13 +45978,13 @@
         <v>9</v>
       </c>
       <c r="K9" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L9" s="34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M9" s="34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -46046,21 +46046,21 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C3" s="36"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="38">
         <v>0</v>
@@ -46068,7 +46068,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="38">
         <v>0</v>
@@ -46076,7 +46076,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B6" s="38">
         <v>0</v>
@@ -46084,7 +46084,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B7" s="38">
         <v>0</v>
@@ -46092,20 +46092,20 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="38">
         <v>0</v>
@@ -46113,7 +46113,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" s="38">
         <v>0</v>
@@ -46121,7 +46121,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="38">
         <v>0</v>
@@ -46129,7 +46129,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="38">
         <v>0</v>
@@ -46137,7 +46137,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -46145,12 +46145,12 @@
         <v>2</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="38">
         <v>0</v>
@@ -46158,7 +46158,7 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" s="38">
         <v>0</v>
@@ -46166,7 +46166,7 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="38" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" s="38">
         <v>0</v>
@@ -46174,7 +46174,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B23" s="38">
         <v>0</v>
@@ -46182,7 +46182,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B24" s="38">
         <v>0</v>
@@ -46190,7 +46190,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" s="38">
         <v>0</v>

</xml_diff>

<commit_message>
Updated System Interfaces tab legend to reflect future state interfaces.
git-svn-id: svn://107.170.10.188:8080/Semoss/trunk@3213 ef391c1c-ee15-45f7-b1d6-dde3d27a2169
</commit_message>
<xml_diff>
--- a/export/Reports/Individual_System_LPNI_Transition_Report_Template.xlsx
+++ b/export/Reports/Individual_System_LPNI_Transition_Report_Template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksmart\workspace64bitNew\SEMOSS_2014\export\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgalbraith\workspace\Semoss\export\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834"/>
+    <workbookView xWindow="240" yWindow="1110" windowWidth="15120" windowHeight="6405" tabRatio="834" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="33" r:id="rId1"/>
@@ -1000,6 +1000,33 @@
     <xf numFmtId="0" fontId="24" fillId="6" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1027,15 +1054,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1045,28 +1063,10 @@
     <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1436,11 +1436,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="421927872"/>
-        <c:axId val="421928264"/>
+        <c:axId val="419553568"/>
+        <c:axId val="419553960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="421927872"/>
+        <c:axId val="419553568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1450,7 +1450,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="421928264"/>
+        <c:crossAx val="419553960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1458,7 +1458,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="421928264"/>
+        <c:axId val="419553960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1469,7 +1469,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="421927872"/>
+        <c:crossAx val="419553568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1602,11 +1602,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="421929048"/>
-        <c:axId val="421929440"/>
+        <c:axId val="297743736"/>
+        <c:axId val="297744128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="421929048"/>
+        <c:axId val="297743736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1616,7 +1616,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="421929440"/>
+        <c:crossAx val="297744128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1624,7 +1624,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="421929440"/>
+        <c:axId val="297744128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1635,7 +1635,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="421929048"/>
+        <c:crossAx val="297743736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1916,11 +1916,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="421930224"/>
-        <c:axId val="421930616"/>
+        <c:axId val="297744912"/>
+        <c:axId val="413011816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="421930224"/>
+        <c:axId val="297744912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1930,7 +1930,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="421930616"/>
+        <c:crossAx val="413011816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1938,7 +1938,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="421930616"/>
+        <c:axId val="413011816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1949,7 +1949,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="421930224"/>
+        <c:crossAx val="297744912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2222,19 +2222,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>772211</xdr:colOff>
+      <xdr:colOff>1028700</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>552188</xdr:rowOff>
+      <xdr:rowOff>522187</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="141" name="Picture 140"/>
+        <xdr:cNvPr id="7" name="Picture 6"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2247,8 +2247,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2009775" y="2324100"/>
-          <a:ext cx="6153836" cy="495038"/>
+          <a:off x="1714500" y="2286000"/>
+          <a:ext cx="6705600" cy="503137"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -44485,7 +44485,7 @@
   </sheetPr>
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:L8"/>
     </sheetView>
   </sheetViews>
@@ -44857,22 +44857,22 @@
     <row r="1" spans="1:13" ht="7.5" customHeight="1"/>
     <row r="2" spans="1:13" s="4" customFormat="1" ht="250.5" customHeight="1">
       <c r="A2" s="3"/>
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="70" t="s">
+      <c r="C2" s="62"/>
+      <c r="D2" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="72"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="65"/>
     </row>
     <row r="3" spans="1:13" s="20" customFormat="1" ht="7.5" customHeight="1">
       <c r="A3" s="16"/>
@@ -44930,22 +44930,22 @@
     </row>
     <row r="7" spans="1:13" s="4" customFormat="1" ht="375" customHeight="1">
       <c r="A7" s="3"/>
-      <c r="B7" s="81" t="s">
+      <c r="B7" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="82"/>
-      <c r="D7" s="70" t="s">
+      <c r="C7" s="62"/>
+      <c r="D7" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="72"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="65"/>
     </row>
     <row r="8" spans="1:13" ht="8.25" customHeight="1">
       <c r="A8" s="5"/>
@@ -44956,112 +44956,112 @@
     </row>
     <row r="9" spans="1:13" s="8" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="7"/>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="62"/>
-      <c r="K9" s="62"/>
-      <c r="L9" s="62"/>
-      <c r="M9" s="63"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="71"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="71"/>
+      <c r="J9" s="71"/>
+      <c r="K9" s="71"/>
+      <c r="L9" s="71"/>
+      <c r="M9" s="72"/>
     </row>
     <row r="10" spans="1:13" s="8" customFormat="1" ht="28.5" customHeight="1">
       <c r="A10" s="7"/>
-      <c r="B10" s="76" t="s">
+      <c r="B10" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76" t="s">
+      <c r="C10" s="66"/>
+      <c r="D10" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="83"/>
-      <c r="F10" s="76" t="s">
+      <c r="E10" s="69"/>
+      <c r="F10" s="66" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="76"/>
-      <c r="H10" s="77" t="s">
+      <c r="G10" s="66"/>
+      <c r="H10" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="78"/>
-      <c r="J10" s="76" t="s">
+      <c r="I10" s="83"/>
+      <c r="J10" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="K10" s="76"/>
-      <c r="L10" s="76" t="s">
+      <c r="K10" s="66"/>
+      <c r="L10" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="76"/>
+      <c r="M10" s="66"/>
     </row>
     <row r="11" spans="1:13" ht="42.75" customHeight="1">
       <c r="A11" s="5"/>
-      <c r="B11" s="79"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="79"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="79"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="79"/>
-      <c r="K11" s="80"/>
-      <c r="L11" s="79"/>
-      <c r="M11" s="80"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="68"/>
+      <c r="L11" s="67"/>
+      <c r="M11" s="68"/>
     </row>
     <row r="13" spans="1:13" ht="16.5">
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="70" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="62"/>
-      <c r="D13" s="62"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="62"/>
-      <c r="H13" s="62"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="63"/>
+      <c r="C13" s="71"/>
+      <c r="D13" s="71"/>
+      <c r="E13" s="71"/>
+      <c r="F13" s="71"/>
+      <c r="G13" s="71"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="71"/>
+      <c r="K13" s="71"/>
+      <c r="L13" s="71"/>
+      <c r="M13" s="72"/>
     </row>
     <row r="14" spans="1:13" ht="51" customHeight="1">
-      <c r="B14" s="67" t="s">
+      <c r="B14" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
-      <c r="H14" s="68"/>
-      <c r="I14" s="68"/>
-      <c r="J14" s="68"/>
-      <c r="K14" s="68"/>
-      <c r="L14" s="68"/>
-      <c r="M14" s="69"/>
+      <c r="C14" s="77"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="77"/>
+      <c r="J14" s="77"/>
+      <c r="K14" s="77"/>
+      <c r="L14" s="77"/>
+      <c r="M14" s="78"/>
     </row>
     <row r="15" spans="1:13">
-      <c r="B15" s="73" t="s">
+      <c r="B15" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="73" t="s">
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="79" t="s">
         <v>60</v>
       </c>
-      <c r="I15" s="74"/>
-      <c r="J15" s="74"/>
-      <c r="K15" s="74"/>
-      <c r="L15" s="74"/>
-      <c r="M15" s="75"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="80"/>
+      <c r="K15" s="80"/>
+      <c r="L15" s="80"/>
+      <c r="M15" s="81"/>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="40"/>
@@ -45288,36 +45288,36 @@
       <c r="M31" s="48"/>
     </row>
     <row r="33" spans="2:13" ht="16.5">
-      <c r="B33" s="61" t="s">
+      <c r="B33" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="62"/>
-      <c r="G33" s="62"/>
-      <c r="H33" s="62"/>
-      <c r="I33" s="62"/>
-      <c r="J33" s="62"/>
-      <c r="K33" s="62"/>
-      <c r="L33" s="62"/>
-      <c r="M33" s="63"/>
+      <c r="C33" s="71"/>
+      <c r="D33" s="71"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+      <c r="H33" s="71"/>
+      <c r="I33" s="71"/>
+      <c r="J33" s="71"/>
+      <c r="K33" s="71"/>
+      <c r="L33" s="71"/>
+      <c r="M33" s="72"/>
     </row>
     <row r="34" spans="2:13" ht="33.75" customHeight="1">
-      <c r="B34" s="64" t="s">
+      <c r="B34" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="65"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="65"/>
-      <c r="K34" s="65"/>
-      <c r="L34" s="65"/>
-      <c r="M34" s="66"/>
+      <c r="C34" s="74"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="74"/>
+      <c r="F34" s="74"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="74"/>
+      <c r="J34" s="74"/>
+      <c r="K34" s="74"/>
+      <c r="L34" s="74"/>
+      <c r="M34" s="75"/>
     </row>
     <row r="35" spans="2:13">
       <c r="B35" s="40"/>
@@ -45545,6 +45545,17 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="B33:M33"/>
+    <mergeCell ref="B34:M34"/>
+    <mergeCell ref="B14:M14"/>
+    <mergeCell ref="D7:M7"/>
+    <mergeCell ref="B9:M9"/>
+    <mergeCell ref="B13:M13"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B4:M4"/>
     <mergeCell ref="D2:M2"/>
@@ -45558,17 +45569,6 @@
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B33:M33"/>
-    <mergeCell ref="B34:M34"/>
-    <mergeCell ref="B14:M14"/>
-    <mergeCell ref="D7:M7"/>
-    <mergeCell ref="B9:M9"/>
-    <mergeCell ref="B13:M13"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -46123,7 +46123,7 @@
   </sheetPr>
   <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="C7" sqref="C7:G7"/>
     </sheetView>
   </sheetViews>

</xml_diff>